<commit_message>
add "danh sach soan hang" page
</commit_message>
<xml_diff>
--- a/Misa_1.xlsx
+++ b/Misa_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VTA-HAN\Desktop\VTA\lotus_warehouse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5FC700-A5CB-4748-85C7-6D2C922492E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9122E6C-6B1E-49E3-B1B1-255F84EF26B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{6D09A305-D742-466F-AD65-26DD6CA8D67C}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$R$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$R$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="63">
   <si>
     <t>K01</t>
   </si>
@@ -195,9 +195,6 @@
   </si>
   <si>
     <t>2022/08+3Y</t>
-  </si>
-  <si>
-    <t>CK2210.0064</t>
   </si>
   <si>
     <t>Nguyễn Thị Hoàng Sinh</t>
@@ -746,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3A838E-AA56-4CD3-B84F-DCA78EDBD6DF}">
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,7 +784,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>5</v>
@@ -802,7 +799,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>9</v>
@@ -826,7 +823,7 @@
         <v>15</v>
       </c>
       <c r="R1" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -840,10 +837,10 @@
         <v>17</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>18</v>
@@ -894,10 +891,10 @@
         <v>27</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>28</v>
@@ -948,10 +945,10 @@
         <v>34</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F4" s="17" t="s">
         <v>28</v>
@@ -1002,10 +999,10 @@
         <v>27</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>18</v>
@@ -1056,10 +1053,10 @@
         <v>34</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F6" s="17" t="s">
         <v>18</v>
@@ -1110,10 +1107,10 @@
         <v>34</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F7" s="17" t="s">
         <v>37</v>
@@ -1264,10 +1261,10 @@
         <v>48</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>28</v>
@@ -1318,10 +1315,10 @@
         <v>50</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>28</v>
@@ -1372,10 +1369,10 @@
         <v>50</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>28</v>
@@ -1415,58 +1412,8 @@
       </c>
       <c r="R12" s="15"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="16">
-        <v>44854</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="J13" s="18">
-        <v>45870</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L13" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M13" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="N13" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="O13" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="P13" s="19">
-        <v>3000</v>
-      </c>
-      <c r="Q13" s="20">
-        <v>0</v>
-      </c>
-      <c r="R13" s="21"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:R13" xr:uid="{9D3A838E-AA56-4CD3-B84F-DCA78EDBD6DF}"/>
+  <autoFilter ref="A1:R12" xr:uid="{9D3A838E-AA56-4CD3-B84F-DCA78EDBD6DF}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>